<commit_message>
[main] Brand new STM32L053R8/Cube1.16.0/Playground/ project.
</commit_message>
<xml_diff>
--- a/doc/Resources/STM32L053R8_Playground.xlsx
+++ b/doc/Resources/STM32L053R8_Playground.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\Nucleo\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\Nucleo\doc\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{780DEF7B-AD37-4333-BD6F-8140BF514EC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25DA087-7FB7-4BD3-B46D-E1C7082F9744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{5898E33E-EB82-47DD-BCC8-15F2BCE71A39}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{5898E33E-EB82-47DD-BCC8-15F2BCE71A39}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder" sheetId="2" r:id="rId1"/>
@@ -524,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0359EFD-2338-4B5B-8135-A1907456F2E5}">
   <dimension ref="B2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -577,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA99893-05EA-430D-BE23-9E5A3816F16D}">
   <dimension ref="B2:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,15 +689,15 @@
         <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>9.86</v>
+        <v>9.85</v>
       </c>
       <c r="E9" s="4">
         <f>D9-C9</f>
-        <v>9.86</v>
+        <v>9.85</v>
       </c>
       <c r="F9" s="6">
         <f>E9/$C$4</f>
-        <v>0.15406249999999999</v>
+        <v>0.15390624999999999</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -752,18 +752,18 @@
       </c>
       <c r="C14" s="4">
         <f>D9</f>
-        <v>9.86</v>
+        <v>9.85</v>
       </c>
       <c r="D14" s="4">
         <v>13.25</v>
       </c>
       <c r="E14" s="4">
         <f>D14-C14</f>
-        <v>3.3900000000000006</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="F14" s="6">
         <f>E14/$C$4</f>
-        <v>5.2968750000000009E-2</v>
+        <v>5.3125000000000006E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[L053R8_NOOS_SYSTEM] Add application system files.
</commit_message>
<xml_diff>
--- a/doc/Resources/STM32L053R8_Playground.xlsx
+++ b/doc/Resources/STM32L053R8_Playground.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\Nucleo\doc\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25DA087-7FB7-4BD3-B46D-E1C7082F9744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650BDEAD-40BF-4750-901A-907AEB3BDF8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{5898E33E-EB82-47DD-BCC8-15F2BCE71A39}"/>
   </bookViews>
@@ -578,7 +578,7 @@
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,7 @@
         <v>1.68</v>
       </c>
       <c r="F8" s="6">
-        <f>E8/$C$3</f>
+        <f>D8/$C$3</f>
         <v>0.21</v>
       </c>
     </row>
@@ -696,7 +696,7 @@
         <v>9.85</v>
       </c>
       <c r="F9" s="6">
-        <f>E9/$C$4</f>
+        <f>D9/$C$4</f>
         <v>0.15390624999999999</v>
       </c>
     </row>
@@ -742,8 +742,8 @@
         <v>0.12000000000000011</v>
       </c>
       <c r="F13" s="6">
-        <f>E13/$C$3</f>
-        <v>1.5000000000000013E-2</v>
+        <f t="shared" ref="F13:F14" si="0">D13/$C$4</f>
+        <v>2.8125000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -755,15 +755,15 @@
         <v>9.85</v>
       </c>
       <c r="D14" s="4">
-        <v>13.25</v>
+        <v>13.81</v>
       </c>
       <c r="E14" s="4">
         <f>D14-C14</f>
-        <v>3.4000000000000004</v>
+        <v>3.9600000000000009</v>
       </c>
       <c r="F14" s="6">
-        <f>E14/$C$4</f>
-        <v>5.3125000000000006E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.21578125000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[L053R8_NOOS_SYSTEM] Update .gitignore and Resources/STM32L053R8_Playground.xlsx
</commit_message>
<xml_diff>
--- a/doc/Resources/STM32L053R8_Playground.xlsx
+++ b/doc/Resources/STM32L053R8_Playground.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\Nucleo\doc\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83FC6AF-0444-47EC-9C49-406F29F029C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCA8057-D817-4924-8641-7A137E515D90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" activeTab="1" xr2:uid="{5898E33E-EB82-47DD-BCC8-15F2BCE71A39}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{5898E33E-EB82-47DD-BCC8-15F2BCE71A39}"/>
   </bookViews>
   <sheets>
     <sheet name="Folder" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Tasks</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Application</t>
   </si>
   <si>
-    <t>System</t>
-  </si>
-  <si>
     <t>app_prd.h</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>app_prd.c</t>
   </si>
   <si>
-    <t>Src</t>
-  </si>
-  <si>
     <t>Include</t>
   </si>
   <si>
@@ -129,6 +123,15 @@
   </si>
   <si>
     <t>Implement APRD basic</t>
+  </si>
+  <si>
+    <t>Periodic</t>
+  </si>
+  <si>
+    <t>feature.h</t>
+  </si>
+  <si>
+    <t>Source</t>
   </si>
 </sst>
 </file>
@@ -533,14 +536,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0359EFD-2338-4B5B-8135-A1907456F2E5}">
   <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -549,39 +552,42 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA99893-05EA-430D-BE23-9E5A3816F16D}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -778,13 +784,13 @@
         <v>3.9600000000000009</v>
       </c>
       <c r="F14" s="6">
-        <f t="shared" ref="F13:F14" si="0">D14/$C$4</f>
+        <f t="shared" ref="F14" si="0">D14/$C$4</f>
         <v>0.21578125000000001</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -840,11 +846,11 @@
         <v>-2.000000000000135E-2</v>
       </c>
       <c r="F19" s="6">
-        <f t="shared" ref="F18:F19" si="1">D19/$C$4</f>
+        <f t="shared" ref="F19" si="1">D19/$C$4</f>
         <v>0.21546874999999999</v>
       </c>
       <c r="G19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -859,7 +865,7 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>